<commit_message>
added some files and just adjusted column width of data files
</commit_message>
<xml_diff>
--- a/wildwood-xlsx-data/survey-scoring.xlsx
+++ b/wildwood-xlsx-data/survey-scoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kswan\Desktop\Year 3 Semester 1\Artificial Intelligence\AI course programming\Projects\project 2\wildwood-csv-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kswan\Desktop\Year 3 Semester 1\Artificial Intelligence\AI course programming\Projects\project 2\wildwood-xlsx-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B008A866-21CA-4531-9DA5-48CD280CC4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40BD625-1C12-4996-B472-DC01D59C0C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="37250" yWindow="-6020" windowWidth="19960" windowHeight="10030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey-scoring" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1057,12 +1057,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" customWidth="1"/>
+    <col min="6" max="6" width="105.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Revert "added some files and just adjusted column width of data files"
This reverts commit 8ace8dceef1c69120e8f55a8ff05b00726ecb515.
</commit_message>
<xml_diff>
--- a/wildwood-xlsx-data/survey-scoring.xlsx
+++ b/wildwood-xlsx-data/survey-scoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kswan\Desktop\Year 3 Semester 1\Artificial Intelligence\AI course programming\Projects\project 2\wildwood-xlsx-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kswan\Desktop\Year 3 Semester 1\Artificial Intelligence\AI course programming\Projects\project 2\wildwood-csv-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40BD625-1C12-4996-B472-DC01D59C0C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B008A866-21CA-4531-9DA5-48CD280CC4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37250" yWindow="-6020" windowWidth="19960" windowHeight="10030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="survey-scoring" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1057,20 +1057,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" customWidth="1"/>
-    <col min="6" max="6" width="105.6328125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>